<commit_message>
More on Final Project
More files relating to my final project have been added.
</commit_message>
<xml_diff>
--- a/Independent Project/Megascops_sampling with subspecies.xlsx
+++ b/Independent Project/Megascops_sampling with subspecies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ab7d75fe672a7f1c/School Work/2024-2025/SPRING 2024/ST GR Bioinformatics - BSC 6932/Bioinformatics_Spring2024/Independent Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="8_{E58127A4-7E4E-4902-9529-08DC5424AC15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9AE935E8-C082-4B6D-92BF-80CDF13D7CB9}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="8_{E58127A4-7E4E-4902-9529-08DC5424AC15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59FA4842-FE26-472A-AFD3-47FA36BB99B8}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{192F87C7-5BD2-734C-9DCC-A3A7405D1862}"/>
   </bookViews>
@@ -365,7 +365,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -385,7 +385,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -405,6 +404,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -727,7 +730,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -772,9 +775,9 @@
         <v>-66.428611000000004</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F2" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" t="s">
         <v>35</v>
       </c>
     </row>
@@ -794,7 +797,7 @@
       <c r="E3" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" t="s">
         <v>36</v>
       </c>
     </row>
@@ -814,7 +817,7 @@
       <c r="E4" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="11" t="s">
         <v>38</v>
       </c>
     </row>
@@ -834,7 +837,7 @@
       <c r="E5" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="11" t="s">
         <v>38</v>
       </c>
     </row>
@@ -854,7 +857,7 @@
       <c r="E6" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="11" t="s">
         <v>38</v>
       </c>
     </row>
@@ -874,7 +877,7 @@
       <c r="E7" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="11" t="s">
         <v>38</v>
       </c>
     </row>
@@ -894,7 +897,7 @@
       <c r="E8" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="11" t="s">
         <v>38</v>
       </c>
     </row>
@@ -914,7 +917,7 @@
       <c r="E9" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="11" t="s">
         <v>37</v>
       </c>
     </row>
@@ -934,7 +937,7 @@
       <c r="E10" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="11" t="s">
         <v>37</v>
       </c>
     </row>
@@ -954,7 +957,7 @@
       <c r="E11" t="s">
         <v>31</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="11" t="s">
         <v>37</v>
       </c>
     </row>
@@ -974,7 +977,7 @@
       <c r="E12" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="F12" s="11" t="s">
         <v>37</v>
       </c>
     </row>
@@ -994,7 +997,7 @@
       <c r="E13" t="s">
         <v>28</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="F13" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1014,7 +1017,7 @@
       <c r="E14" t="s">
         <v>28</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="11" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1034,7 +1037,7 @@
       <c r="E15" t="s">
         <v>28</v>
       </c>
-      <c r="F15" s="12" t="s">
+      <c r="F15" s="11" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1054,7 +1057,7 @@
       <c r="E16" t="s">
         <v>28</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="F16" s="11" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1074,7 +1077,7 @@
       <c r="E17" t="s">
         <v>29</v>
       </c>
-      <c r="F17" s="12" t="s">
+      <c r="F17" s="11" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1094,7 +1097,7 @@
       <c r="E18" t="s">
         <v>29</v>
       </c>
-      <c r="F18" s="12" t="s">
+      <c r="F18" s="11" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1114,7 +1117,7 @@
       <c r="E19" t="s">
         <v>29</v>
       </c>
-      <c r="F19" s="12" t="s">
+      <c r="F19" s="11" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1134,7 +1137,7 @@
       <c r="E20" t="s">
         <v>28</v>
       </c>
-      <c r="F20" s="12" t="s">
+      <c r="F20" s="11" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1154,7 +1157,7 @@
       <c r="E21" t="s">
         <v>28</v>
       </c>
-      <c r="F21" s="12" t="s">
+      <c r="F21" s="11" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1174,7 +1177,7 @@
       <c r="E22" t="s">
         <v>29</v>
       </c>
-      <c r="F22" s="13" t="s">
+      <c r="F22" s="12" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>